<commit_message>
Worked on Garage and Vehicles
</commit_message>
<xml_diff>
--- a/Design/Burndown Chart.xlsx
+++ b/Design/Burndown Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB8E8910-D91A-464B-9BFE-2CFB31DC6E66}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB53D1B4-6488-4817-AAEE-2DCC870A390C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="336" windowWidth="20736" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +130,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,14 +160,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -437,7 +452,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -463,7 +478,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B3">
@@ -471,7 +486,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B4">
@@ -479,7 +494,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5">
@@ -487,7 +502,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B6">
@@ -495,7 +510,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7">
@@ -535,7 +550,7 @@
       <c r="G9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="M9" t="s">
@@ -555,7 +570,7 @@
       <c r="G10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="M10" t="s">

</xml_diff>

<commit_message>
Added Javadoc & UML Class Diagram
</commit_message>
<xml_diff>
--- a/Design/Burndown Chart.xlsx
+++ b/Design/Burndown Chart.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0A64DB-9FCD-4E8A-9689-38F37B87D767}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DF9106-F796-4850-A574-0671CF71E3D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="336" windowWidth="20736" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>Tasks</t>
   </si>
@@ -455,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -467,7 +467,7 @@
     <col min="2" max="2" width="30.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -483,7 +483,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -491,7 +491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
@@ -507,7 +507,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
@@ -515,27 +515,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
@@ -543,85 +531,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="G9" s="1"/>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14">
         <f>SUM(B2:B12)</f>
         <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F17" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>